<commit_message>
Replaced templates (user ones with no metadata)
</commit_message>
<xml_diff>
--- a/services/src/main/resources/files/template.xlsx
+++ b/services/src/main/resources/files/template.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="15180" windowHeight="5265"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -23,6 +23,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -50,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -63,9 +64,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -103,7 +104,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -175,7 +176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>

</xml_diff>

<commit_message>
Add excel new sheet label
</commit_message>
<xml_diff>
--- a/services/src/main/resources/files/template.xlsx
+++ b/services/src/main/resources/files/template.xlsx
@@ -1,32 +1,33 @@
 
 <file path=META-INF/manifest.xml><?xml version="1.0" encoding="utf-8"?>
-<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.2">
-  <manifest:file-entry manifest:full-path="/" manifest:version="1.2" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
-  <manifest:file-entry manifest:full-path="Thumbnails/thumbnail.png" manifest:media-type="image/png"/>
+<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.3">
+  <manifest:file-entry manifest:full-path="/" manifest:version="1.3" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
   <manifest:file-entry manifest:full-path="Configurations2/" manifest:media-type="application/vnd.sun.xml.ui.configuration"/>
-  <manifest:file-entry manifest:full-path="content.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
   <manifest:file-entry manifest:full-path="meta.xml" manifest:media-type="text/xml"/>
   <manifest:file-entry manifest:full-path="styles.xml" manifest:media-type="text/xml"/>
-  <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
+  <manifest:file-entry manifest:full-path="content.xml" manifest:media-type="text/xml"/>
   <manifest:file-entry manifest:full-path="settings.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="Thumbnails/thumbnail.png" manifest:media-type="image/png"/>
 </manifest:manifest>
 </file>
 
 <file path=content.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-content xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
+<office:document-content xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xforms="http://www.w3.org/2002/xforms" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Noto Sans Mono CJK JP" svg:font-family="'Noto Sans Mono CJK JP'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="59.75pt"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.108cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
-      <style:table-row-properties style:row-height="15pt" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.487cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -39,12 +40,12 @@
       </table:calculation-settings>
       <table:table table:name="Sheet1" table:style-name="ta1">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="1024" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="64" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1" table:number-rows-repeated="1048575">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell table:number-columns-repeated="64"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell table:number-columns-repeated="64"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -54,13 +55,13 @@
 </file>
 
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
+<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2020-01-30T11:34:53</meta:creation-date>
-    <dc:date>2020-12-22T12:30:32.892155552</dc:date>
-    <meta:editing-duration>PT4M4S</meta:editing-duration>
-    <meta:editing-cycles>3</meta:editing-cycles>
-    <meta:generator>LibreOffice/6.0.7.3$Linux_X86_64 LibreOffice_project/00m0$Build-3</meta:generator>
+    <dc:date>2020-12-25T14:29:12.944445125</dc:date>
+    <meta:editing-duration>PT4M27S</meta:editing-duration>
+    <meta:editing-cycles>4</meta:editing-cycles>
+    <meta:generator>LibreOffice/7.0.3.1$Linux_X86_64 LibreOffice_project/00$Build-1</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="0" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">14.0300</meta:user-defined>
     <meta:user-defined meta:name="DocSecurity" meta:value-type="float">0</meta:user-defined>
@@ -73,20 +74,20 @@
 </file>
 
 <file path=settings.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:ooo="http://openoffice.org/2004/office" office:version="1.2">
+<office:document-settings xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">2107</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">529</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">486</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">10</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">7</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">8</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -104,7 +105,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1245</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1235</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -112,7 +113,7 @@
           <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-          <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
+          <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
           <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
@@ -130,123 +131,130 @@
       </config:config-item-map-indexed>
     </config:config-item-set>
     <config:config-item-set config:name="ooo:configuration-settings">
+      <config:config-item config:name="EmbedComplexScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedAsianScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
+      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
+      <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
+      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
-      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
+      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
-      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
-      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
-      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
-      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
-      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
-      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
       <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
+      <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
+      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
+      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
 </file>
 
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-styles xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
+<office:document-styles xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" office:version="1.3">
   <office:font-face-decls>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Noto Sans Mono CJK JP" svg:font-family="'Noto Sans Mono CJK JP'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:styles>
     <style:default-style style:family="table-cell">
-      <style:paragraph-properties style:tab-stop-distance="36pt"/>
-      <style:text-properties style:font-name="Liberation Sans" fo:language="en" fo:country="US" style:font-name-asian="DejaVu Sans" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="DejaVu Sans" style:language-complex="hi" style:country-complex="IN"/>
+      <style:paragraph-properties style:tab-stop-distance="1.27cm"/>
+      <style:text-properties style:font-name="Liberation Sans" fo:language="zxx" fo:country="none" style:font-name-asian="DejaVu Sans" style:language-asian="zxx" style:country-asian="none" style:font-name-complex="DejaVu Sans" style:language-complex="zxx" style:country-complex="none"/>
     </style:default-style>
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:time-style style:name="N121">
+    <number:time-style style:name="N111">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N122" number:truncate-on-overflow="false">
+    <number:time-style style:name="N112" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N123">
+    <number:time-style style:name="N113">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N124">
-      <number:scientific-number number:decimal-places="1" loext:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" loext:exponent-interval="3" loext:forced-exponent-sign="true"/>
+    <number:number-style style:name="N114">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <number:currency-style style:name="N10122P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10122" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10122P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10123P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10123" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10123P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10125P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10125" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10125P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10126P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10126" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10126P0"/>
     </number:currency-style>
@@ -314,43 +322,43 @@
       <number:minutes number:style="long"/>
     </number:date-style>
     <number:number-style style:name="N10137P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10137" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10137P0"/>
     </number:number-style>
     <number:number-style style:name="N10139P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10139" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10139P0"/>
     </number:number-style>
     <number:number-style style:name="N10143P0" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10143P1" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N10143P2" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:number-style>
     <number:text-style style:name="N10143" number:language="en" number:country="US">
@@ -363,20 +371,20 @@
     </number:text-style>
     <number:currency-style style:name="N10147P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10147P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N10147P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
+      <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:currency-style>
     <number:text-style style:name="N10147" number:language="en" number:country="US">
@@ -388,23 +396,23 @@
       <style:map style:condition="value()=0" style:apply-style-name="N10147P2"/>
     </number:text-style>
     <number:number-style style:name="N10151P0" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10151P1" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N10151P2" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
     <number:text-style style:name="N10151" number:language="en" number:country="US">
@@ -417,22 +425,22 @@
     </number:text-style>
     <number:currency-style style:name="N10155P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10155P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N10155P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
+      <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:text-style style:name="N10155" number:language="en" number:country="US">
@@ -501,26 +509,29 @@
     <style:style style:name="Accent_20_3" style:display-name="Accent 3" style:family="table-cell" style:parent-style-name="Accent">
       <style:table-cell-properties fo:background-color="#dddddd"/>
     </style:style>
+    <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="10pt" fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="#000000" fo:font-weight="bold"/>
+    </style:style>
   </office:styles>
   <office:automatic-styles>
     <style:page-layout style:name="Mpm1">
       <style:page-layout-properties style:first-page-number="continue" style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-bottom="7.09pt"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm"/>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-top="7.09pt"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm"/>
       </style:footer-style>
     </style:page-layout>
     <style:page-layout style:name="Mpm2">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-bottom="7.09pt" fo:border="2.49pt solid #000000" fo:padding="0.51pt" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-top="7.09pt" fo:border="2.49pt solid #000000" fo:padding="0.51pt" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:footer-style>
@@ -555,9 +566,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2020-12-22">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2020-12-25">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="12:30:00.044066858">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="14:28:49.114648599">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
TASK-37045: Update languages of default documents for onlyOffice (#71)
</commit_message>
<xml_diff>
--- a/services/src/main/resources/files/template.xlsx
+++ b/services/src/main/resources/files/template.xlsx
@@ -1,32 +1,33 @@
 
 <file path=META-INF/manifest.xml><?xml version="1.0" encoding="utf-8"?>
-<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.2">
-  <manifest:file-entry manifest:full-path="/" manifest:version="1.2" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
-  <manifest:file-entry manifest:full-path="Thumbnails/thumbnail.png" manifest:media-type="image/png"/>
+<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.3">
+  <manifest:file-entry manifest:full-path="/" manifest:version="1.3" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
   <manifest:file-entry manifest:full-path="Configurations2/" manifest:media-type="application/vnd.sun.xml.ui.configuration"/>
-  <manifest:file-entry manifest:full-path="content.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
   <manifest:file-entry manifest:full-path="meta.xml" manifest:media-type="text/xml"/>
   <manifest:file-entry manifest:full-path="styles.xml" manifest:media-type="text/xml"/>
-  <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
+  <manifest:file-entry manifest:full-path="content.xml" manifest:media-type="text/xml"/>
   <manifest:file-entry manifest:full-path="settings.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="Thumbnails/thumbnail.png" manifest:media-type="image/png"/>
 </manifest:manifest>
 </file>
 
 <file path=content.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-content xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
+<office:document-content xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xforms="http://www.w3.org/2002/xforms" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Noto Sans Mono CJK JP" svg:font-family="'Noto Sans Mono CJK JP'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="59.75pt"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.108cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
-      <style:table-row-properties style:row-height="15pt" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.487cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -39,12 +40,12 @@
       </table:calculation-settings>
       <table:table table:name="Sheet1" table:style-name="ta1">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="1024" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="64" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1" table:number-rows-repeated="1048575">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell table:number-columns-repeated="64"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell table:number-columns-repeated="64"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -54,13 +55,13 @@
 </file>
 
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
+<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2020-01-30T11:34:53</meta:creation-date>
-    <dc:date>2020-12-22T12:30:32.892155552</dc:date>
-    <meta:editing-duration>PT4M4S</meta:editing-duration>
-    <meta:editing-cycles>3</meta:editing-cycles>
-    <meta:generator>LibreOffice/6.0.7.3$Linux_X86_64 LibreOffice_project/00m0$Build-3</meta:generator>
+    <dc:date>2020-12-25T14:29:12.944445125</dc:date>
+    <meta:editing-duration>PT4M27S</meta:editing-duration>
+    <meta:editing-cycles>4</meta:editing-cycles>
+    <meta:generator>LibreOffice/7.0.3.1$Linux_X86_64 LibreOffice_project/00$Build-1</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="0" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">14.0300</meta:user-defined>
     <meta:user-defined meta:name="DocSecurity" meta:value-type="float">0</meta:user-defined>
@@ -73,20 +74,20 @@
 </file>
 
 <file path=settings.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:ooo="http://openoffice.org/2004/office" office:version="1.2">
+<office:document-settings xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">2107</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">529</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">486</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">10</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">7</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">8</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -104,7 +105,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1245</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1235</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -112,7 +113,7 @@
           <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-          <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
+          <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
           <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
@@ -130,123 +131,130 @@
       </config:config-item-map-indexed>
     </config:config-item-set>
     <config:config-item-set config:name="ooo:configuration-settings">
+      <config:config-item config:name="EmbedComplexScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedAsianScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
+      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
+      <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
+      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
-      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
+      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
-      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
-      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
-      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
-      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
-      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
-      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
       <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
+      <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
+      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
+      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
 </file>
 
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-styles xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
+<office:document-styles xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:rpt="http://openoffice.org/2005/report" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" office:version="1.3">
   <office:font-face-decls>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Noto Sans Mono CJK JP" svg:font-family="'Noto Sans Mono CJK JP'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:styles>
     <style:default-style style:family="table-cell">
-      <style:paragraph-properties style:tab-stop-distance="36pt"/>
-      <style:text-properties style:font-name="Liberation Sans" fo:language="en" fo:country="US" style:font-name-asian="DejaVu Sans" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="DejaVu Sans" style:language-complex="hi" style:country-complex="IN"/>
+      <style:paragraph-properties style:tab-stop-distance="1.27cm"/>
+      <style:text-properties style:font-name="Liberation Sans" fo:language="zxx" fo:country="none" style:font-name-asian="DejaVu Sans" style:language-asian="zxx" style:country-asian="none" style:font-name-complex="DejaVu Sans" style:language-complex="zxx" style:country-complex="none"/>
     </style:default-style>
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:time-style style:name="N121">
+    <number:time-style style:name="N111">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N122" number:truncate-on-overflow="false">
+    <number:time-style style:name="N112" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N123">
+    <number:time-style style:name="N113">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N124">
-      <number:scientific-number number:decimal-places="1" loext:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" loext:exponent-interval="3" loext:forced-exponent-sign="true"/>
+    <number:number-style style:name="N114">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <number:currency-style style:name="N10122P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10122" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10122P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10123P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10123" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10123P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10125P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10125" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10125P0"/>
     </number:currency-style>
     <number:currency-style style:name="N10126P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10126" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10126P0"/>
     </number:currency-style>
@@ -314,43 +322,43 @@
       <number:minutes number:style="long"/>
     </number:date-style>
     <number:number-style style:name="N10137P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10137" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10137P0"/>
     </number:number-style>
     <number:number-style style:name="N10139P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10139" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N10139P0"/>
     </number:number-style>
     <number:number-style style:name="N10143P0" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10143P1" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N10143P2" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:number-style>
     <number:text-style style:name="N10143" number:language="en" number:country="US">
@@ -363,20 +371,20 @@
     </number:text-style>
     <number:currency-style style:name="N10147P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10147P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N10147P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
+      <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:currency-style>
     <number:text-style style:name="N10147" number:language="en" number:country="US">
@@ -388,23 +396,23 @@
       <style:map style:condition="value()=0" style:apply-style-name="N10147P2"/>
     </number:text-style>
     <number:number-style style:name="N10151P0" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N10151P1" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N10151P2" style:volatile="true" number:language="en" number:country="US">
-      <loext:text> </loext:text>
-      <loext:fill-character> </loext:fill-character>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
     <number:text-style style:name="N10151" number:language="en" number:country="US">
@@ -417,22 +425,22 @@
     </number:text-style>
     <number:currency-style style:name="N10155P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N10155P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N10155P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
-      <loext:fill-character> </loext:fill-character>
+      <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:text-style style:name="N10155" number:language="en" number:country="US">
@@ -501,26 +509,29 @@
     <style:style style:name="Accent_20_3" style:display-name="Accent 3" style:family="table-cell" style:parent-style-name="Accent">
       <style:table-cell-properties fo:background-color="#dddddd"/>
     </style:style>
+    <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="10pt" fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="#000000" fo:font-weight="bold"/>
+    </style:style>
   </office:styles>
   <office:automatic-styles>
     <style:page-layout style:name="Mpm1">
       <style:page-layout-properties style:first-page-number="continue" style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-bottom="7.09pt"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm"/>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-top="7.09pt"/>
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm"/>
       </style:footer-style>
     </style:page-layout>
     <style:page-layout style:name="Mpm2">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-bottom="7.09pt" fo:border="2.49pt solid #000000" fo:padding="0.51pt" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-bottom="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="21.26pt" fo:margin-left="0pt" fo:margin-right="0pt" fo:margin-top="7.09pt" fo:border="2.49pt solid #000000" fo:padding="0.51pt" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.75cm" fo:margin-left="0cm" fo:margin-right="0cm" fo:margin-top="0.25cm" fo:border="2.49pt solid #000000" fo:padding="0.018cm" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:footer-style>
@@ -555,9 +566,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2020-12-22">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2020-12-25">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="12:30:00.044066858">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="14:28:49.114648599">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>